<commit_message>
add D_h,D_heel,D_yaw to sailbot_library.slx and update excel sheet
</commit_message>
<xml_diff>
--- a/Simulink_models/block_responsibility_sheet.xlsx
+++ b/Simulink_models/block_responsibility_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brucecui\OneDrive\work\UBC\SailBots\boat-simulator\Simulink_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_F25DC773A252ABDACC10487E29595CBE5ADE58EB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B08DD45A-24B6-4FEB-94A2-09B6D07531B5}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC10487E29595CBE5ADE58EB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D3C4B3F2-E9B4-4D8A-8948-DC3C00593E89}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>V_dot</t>
   </si>
@@ -420,7 +420,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,6 +486,9 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -494,6 +497,9 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -502,6 +508,9 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -518,6 +527,9 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -526,6 +538,9 @@
       <c r="E12" t="s">
         <v>15</v>
       </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -533,6 +548,9 @@
       </c>
       <c r="E13" t="s">
         <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add C_a and C_rb to sailbot_library
</commit_message>
<xml_diff>
--- a/Simulink_models/block_responsibility_sheet.xlsx
+++ b/Simulink_models/block_responsibility_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brucecui\OneDrive\work\UBC\SailBots\boat-simulator\Simulink_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlum1\Documents\boat-simulator\Simulink_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC10487E29595CBE5ADE58EB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D3C4B3F2-E9B4-4D8A-8948-DC3C00593E89}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D001B2-BB1C-466F-9A83-E9AA91851249}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>V_dot</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -420,12 +423,12 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -436,12 +439,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -452,7 +455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -463,7 +466,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -474,12 +477,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -490,7 +493,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -501,7 +504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -512,7 +515,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -520,7 +523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -531,7 +534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -542,7 +545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -553,7 +556,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -561,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -569,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -577,28 +580,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>17</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add v_ and alpha_ values. Also add J to library
</commit_message>
<xml_diff>
--- a/Simulink_models/block_responsibility_sheet.xlsx
+++ b/Simulink_models/block_responsibility_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlum1\Documents\boat-simulator\Simulink_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brucecui\OneDrive\work\UBC\SailBots\boat-simulator\Simulink_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D001B2-BB1C-466F-9A83-E9AA91851249}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE1F2E-2D79-4C0E-97FA-D89249A1F7E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>V_dot</t>
   </si>
@@ -103,6 +103,36 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>v_aw</t>
+  </si>
+  <si>
+    <t>v_alpha_aw</t>
+  </si>
+  <si>
+    <t>v_ar</t>
+  </si>
+  <si>
+    <t>alpha_ar</t>
+  </si>
+  <si>
+    <t>v_ak</t>
+  </si>
+  <si>
+    <t>alpha_ak</t>
+  </si>
+  <si>
+    <t>v_ah</t>
+  </si>
+  <si>
+    <t>alpha_ah</t>
   </si>
 </sst>
 </file>
@@ -420,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -439,12 +469,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -455,7 +485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -466,7 +496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -477,12 +507,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -493,7 +523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -504,7 +534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -515,7 +545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -523,93 +553,146 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E21" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E22" t="s">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="G25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="G20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="G30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>17</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C32" t="s">
         <v>8</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G32" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>